<commit_message>
Date: 29 Dec 2025
</commit_message>
<xml_diff>
--- a/MySeleniumProject/ExcelFiles/OHRMLoginData.xlsx
+++ b/MySeleniumProject/ExcelFiles/OHRMLoginData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StarAgile\Demos\SA2509016\MySeleniumProject\ExcelFiles\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>User Name</t>
   </si>
@@ -41,9 +41,6 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>Not Run</t>
-  </si>
-  <si>
     <t>shashikant</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Message</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>bhagya</t>
   </si>
   <si>
@@ -77,27 +71,68 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Pawan Mankar</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
     <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>manda user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="17"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,8 +155,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,121 +447,121 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>